<commit_message>
New control, new results
</commit_message>
<xml_diff>
--- a/Data_Raw/general/country_agriculture_output.xlsx
+++ b/Data_Raw/general/country_agriculture_output.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boblin\Documents\GitHub\Taiwan_Land\Data_Raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BobLin\GitHub\Taiwan_Land\Data_Raw\general\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4F992D-DB62-46F2-8806-5DB8B6B82FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80E7B3A-D912-4D4F-A102-FB22218908A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="15196" xr2:uid="{A6D0FDC5-CAD0-4EB4-B6AC-8E7D69AF37AC}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{A6D0FDC5-CAD0-4EB4-B6AC-8E7D69AF37AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,30 +35,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
-    <t>Sum</t>
+    <t>Total Value</t>
   </si>
   <si>
-    <t>Average</t>
+    <t>Rice Value</t>
   </si>
   <si>
-    <t>Running Total</t>
+    <t>Common Crop Value (exclude Rice)</t>
   </si>
   <si>
-    <t>Count</t>
+    <t>Special Crop Value</t>
   </si>
   <si>
-    <t>Total_Value</t>
+    <t>Horticultural Crop Value</t>
   </si>
   <si>
-    <t>Common_Crop_Value</t>
+    <t>Livestock Value</t>
   </si>
   <si>
-    <t>Special_Crop_Value</t>
+    <t>Common Crop Value</t>
   </si>
   <si>
-    <t>Horticultural_Crop_Value</t>
+    <t>Sericulture Value</t>
   </si>
 </sst>
 </file>
@@ -157,7 +157,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -171,13 +171,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Taiwan Agricultural Output</a:t>
+              <a:t>Taiwan Agricultural Output by Types (NT$ million)</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> ($NT millions)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -194,7 +189,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -213,8 +208,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -225,29 +220,55 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Total_Value</c:v>
+                  <c:v>Rice Value</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$19:$A$32</c:f>
+              <c:f>Sheet1!$A$19:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1950</c:v>
                 </c:pt>
@@ -268,86 +289,43 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1956</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1957</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1958</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1959</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1960</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1961</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1962</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1963</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$B$32</c:f>
+              <c:f>Sheet1!$B$19:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2786.7528339999999</c:v>
+                  <c:v>1255.12095</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3773.7650530000001</c:v>
+                  <c:v>1507.6941039999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5837.5524180000002</c:v>
+                  <c:v>2932.9228010000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8681.4118269999999</c:v>
+                  <c:v>4577.1817259999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7430.6435419999998</c:v>
+                  <c:v>3531.8329450000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9494.8602339999998</c:v>
+                  <c:v>4357.2195009999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10574.045432000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12390.940296999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>13709.273168</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>15611.829655</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20659.549781999998</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>23186.682767999999</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>23406.352095999999</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>24508.034204</c:v>
+                  <c:v>4786.005365</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3506-45D3-9C44-A2F61EADAD5A}"/>
+              <c16:uniqueId val="{00000000-3830-4A21-A172-C98ADA1C537F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -360,29 +338,55 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Common_Crop_Value</c:v>
+                  <c:v>Common Crop Value (exclude Rice)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$19:$A$32</c:f>
+              <c:f>Sheet1!$A$19:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1950</c:v>
                 </c:pt>
@@ -403,86 +407,43 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1956</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1957</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1958</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1959</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1960</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1961</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1962</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1963</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$32</c:f>
+              <c:f>Sheet1!$C$19:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1553.185796</c:v>
+                  <c:v>298.06484599999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1925.545314</c:v>
+                  <c:v>417.85120999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3596.1844769999998</c:v>
+                  <c:v>663.26167599999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5379.7804310000001</c:v>
+                  <c:v>802.598705</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4392.9813219999996</c:v>
+                  <c:v>861.14837699999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5463.5659850000002</c:v>
+                  <c:v>1106.3464839999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6117.3616760000004</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6924.7113810000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7483.340099</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7979.6766719999996</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11997.894672</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>13127.507981999999</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12809.779477</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>12650.218746</c:v>
+                  <c:v>1331.356311</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3506-45D3-9C44-A2F61EADAD5A}"/>
+              <c16:uniqueId val="{00000001-3830-4A21-A172-C98ADA1C537F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -495,29 +456,55 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Special_Crop_Value</c:v>
+                  <c:v>Special Crop Value</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$19:$A$32</c:f>
+              <c:f>Sheet1!$A$19:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1950</c:v>
                 </c:pt>
@@ -538,37 +525,16 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1956</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1957</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1958</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1959</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1960</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1961</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1962</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1963</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$19:$D$32</c:f>
+              <c:f>Sheet1!$D$19:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>523.64871600000004</c:v>
                 </c:pt>
@@ -589,35 +555,13 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1782.4282450000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2188.6539240000002</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2336.585079</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2800.7758260000001</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2863.7095049999998</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3471.7221920000002</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3327.1984940000002</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3707.2760069999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-3506-45D3-9C44-A2F61EADAD5A}"/>
+              <c16:uniqueId val="{00000002-3830-4A21-A172-C98ADA1C537F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -630,29 +574,58 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Horticultural_Crop_Value</c:v>
+                  <c:v>Horticultural Crop Value</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$19:$A$32</c:f>
+              <c:f>Sheet1!$A$19:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1950</c:v>
                 </c:pt>
@@ -673,37 +646,16 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1956</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1957</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1958</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1959</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1960</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1961</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1962</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1963</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$19:$E$32</c:f>
+              <c:f>Sheet1!$E$19:$E$25</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>297.153074</c:v>
                 </c:pt>
@@ -724,35 +676,255 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>694.92077400000005</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>837.60674800000004</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1164.379666</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1338.886027</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1618.128584</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1724.2173439999999</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1995.738863</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2690.6313230000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-3506-45D3-9C44-A2F61EADAD5A}"/>
+              <c16:uniqueId val="{00000003-3830-4A21-A172-C98ADA1C537F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sericulture Value</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$19:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1951</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1952</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1953</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1954</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1955</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1956</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$19:$F$25</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.22844800000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.28353600000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.79500400000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1640470000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1197649999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2695720000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.4998899999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-3830-4A21-A172-C98ADA1C537F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Livestock Value</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$19:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1951</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1952</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1953</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1954</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1955</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1956</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$19:$G$25</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>412.53680000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>676.08507499999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>841.10987899999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1209.9489739999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1356.111251</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1775.6815300000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1974.8348470000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-3830-4A21-A172-C98ADA1C537F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -764,24 +936,23 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="310810176"/>
-        <c:axId val="310808096"/>
-      </c:lineChart>
+        <c:axId val="1444290927"/>
+        <c:axId val="1444291759"/>
+      </c:areaChart>
       <c:catAx>
-        <c:axId val="310810176"/>
+        <c:axId val="1444290927"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -812,7 +983,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="310808096"/>
+        <c:crossAx val="1444291759"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -820,7 +991,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="310808096"/>
+        <c:axId val="1444291759"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -871,9 +1042,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="310810176"/>
+        <c:crossAx val="1444290927"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -915,14 +1086,7 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
+    <c:dispBlanksAs val="zero"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -959,13 +1123,10 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -999,7 +1160,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="346">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1010,7 +1171,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -1023,7 +1184,7 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
@@ -1040,7 +1201,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1056,7 +1217,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -1100,45 +1261,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1150,31 +1301,29 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -1278,14 +1427,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -1375,20 +1518,20 @@
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -1401,6 +1544,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1432,7 +1586,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1441,14 +1595,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1502,14 +1655,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1518,23 +1665,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>359567</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>544830</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>481011</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AED39BE3-DFB9-42F9-BE46-6DBEF21A0C61}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC9522EB-A72E-4AC6-814E-ACC95E659CD5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1852,579 +1999,638 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAA5E437-CE35-4807-A90F-BD0461C1805A}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="17.1328125" customWidth="1"/>
-    <col min="3" max="3" width="18.53125" customWidth="1"/>
-    <col min="4" max="4" width="15.1328125" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="2" max="2" width="17.1015625" customWidth="1"/>
+    <col min="3" max="3" width="18.5234375" customWidth="1"/>
+    <col min="4" max="4" width="15.1015625" customWidth="1"/>
+    <col min="5" max="5" width="18.734375" customWidth="1"/>
+    <col min="6" max="7" width="24.26171875" customWidth="1"/>
+    <col min="8" max="8" width="16.3671875" customWidth="1"/>
+    <col min="10" max="10" width="28.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2">
         <v>1950</v>
       </c>
       <c r="B2" s="1">
+        <f ca="1">SUM(C2:H2)</f>
         <v>2786752834</v>
       </c>
       <c r="C2" s="1">
+        <f ca="1">SUM(INDIRECT(CONCATENATE("'[rice.xlsx]", A2, "'!$E$2:$E$45")))</f>
+        <v>1255120950</v>
+      </c>
+      <c r="D2" s="1">
+        <f ca="1">SUM(INDIRECT(CONCATENATE("'[general_value.xlsx]", A2, "'!$C$2:$C$23")))-C2</f>
+        <v>298064846</v>
+      </c>
+      <c r="E2" s="1">
+        <f ca="1">SUM(INDIRECT(CONCATENATE("'[general_value.xlsx]", A2, "'!$D$2:$D$23")))</f>
+        <v>523648716</v>
+      </c>
+      <c r="F2" s="1">
+        <f ca="1">SUM(INDIRECT(CONCATENATE("'[general_value.xlsx]", A2, "'!$E$2:$E$23")))</f>
+        <v>297153074</v>
+      </c>
+      <c r="G2" s="1">
+        <f ca="1">SUM(INDIRECT(CONCATENATE("'[general_value.xlsx]", A2, "'!$F$2:$F$23")))</f>
+        <v>228448</v>
+      </c>
+      <c r="H2">
+        <f ca="1">SUM(INDIRECT(CONCATENATE("'[general_value.xlsx]", A2, "'!$G$2:$G$23")))</f>
+        <v>412536800</v>
+      </c>
+      <c r="J2" s="1">
         <v>1553185796</v>
       </c>
-      <c r="D2" s="1">
-        <v>523648716</v>
-      </c>
-      <c r="E2" s="1">
-        <v>297153074</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>1951</v>
       </c>
       <c r="B3" s="1">
+        <f t="shared" ref="B3:B8" ca="1" si="0">SUM(C3:H3)</f>
         <v>3773765053</v>
       </c>
       <c r="C3" s="1">
+        <f t="shared" ref="C3:C8" ca="1" si="1">SUM(INDIRECT(CONCATENATE("'[rice.xlsx]", A3, "'!$E$2:$E$45")))</f>
+        <v>1507694104</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D8" ca="1" si="2">SUM(INDIRECT(CONCATENATE("'[general_value.xlsx]", A3, "'!$C$2:$C$23")))-C3</f>
+        <v>417851210</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E8" ca="1" si="3">SUM(INDIRECT(CONCATENATE("'[general_value.xlsx]", A3, "'!$D$2:$D$23")))</f>
+        <v>748338763</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" ref="F3:F8" ca="1" si="4">SUM(INDIRECT(CONCATENATE("'[general_value.xlsx]", A3, "'!$E$2:$E$23")))</f>
+        <v>423512365</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" ref="G3:G8" ca="1" si="5">SUM(INDIRECT(CONCATENATE("'[general_value.xlsx]", A3, "'!$F$2:$F$23")))</f>
+        <v>283536</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H8" ca="1" si="6">SUM(INDIRECT(CONCATENATE("'[general_value.xlsx]", A3, "'!$G$2:$G$23")))</f>
+        <v>676085075</v>
+      </c>
+      <c r="J3" s="1">
         <v>1925545314</v>
       </c>
-      <c r="D3" s="1">
-        <v>748338763</v>
-      </c>
-      <c r="E3" s="1">
-        <v>423512365</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2">
         <v>1952</v>
       </c>
       <c r="B4" s="1">
+        <f t="shared" ca="1" si="0"/>
         <v>5837552418</v>
       </c>
       <c r="C4" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>2932922801</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>663261676</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>983552005</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>415911053</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>795004</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ca="1" si="6"/>
+        <v>841109879</v>
+      </c>
+      <c r="J4" s="1">
         <v>3596184477</v>
       </c>
-      <c r="D4" s="1">
-        <v>983552005</v>
-      </c>
-      <c r="E4" s="1">
-        <v>415911053</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>1953</v>
       </c>
       <c r="B5" s="1">
+        <f t="shared" ca="1" si="0"/>
         <v>8681411827</v>
       </c>
       <c r="C5" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>4577181726</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>802598705</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>1638025677</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>452492698</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>1164047</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ca="1" si="6"/>
+        <v>1209948974</v>
+      </c>
+      <c r="J5" s="1">
         <v>5379780431</v>
       </c>
-      <c r="D5" s="1">
-        <v>1638025677</v>
-      </c>
-      <c r="E5" s="1">
-        <v>452492698</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2">
         <v>1954</v>
       </c>
       <c r="B6" s="1">
+        <f t="shared" ca="1" si="0"/>
         <v>7430643542</v>
       </c>
       <c r="C6" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>3531832945</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>861148377</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>1169623886</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>510807318</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>1119765</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ca="1" si="6"/>
+        <v>1356111251</v>
+      </c>
+      <c r="J6" s="1">
         <v>4392981322</v>
       </c>
-      <c r="D6" s="1">
-        <v>1169623886</v>
-      </c>
-      <c r="E6" s="1">
-        <v>510807318</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>1955</v>
       </c>
       <c r="B7" s="1">
+        <f t="shared" ca="1" si="0"/>
         <v>9494860234</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>4357219501</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>1106346484</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>1623182115</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>630161032</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>2269572</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ca="1" si="6"/>
+        <v>1775681530</v>
+      </c>
+      <c r="J7" s="3">
         <v>5463565985</v>
       </c>
-      <c r="D7" s="1">
-        <v>1623182115</v>
-      </c>
-      <c r="E7" s="1">
-        <v>630161032</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2">
         <v>1956</v>
       </c>
       <c r="B8" s="1">
+        <f t="shared" ca="1" si="0"/>
         <v>10574045432</v>
       </c>
       <c r="C8" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>4786005365</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>1331356311</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>1782428245</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>694920774</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>4499890</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ca="1" si="6"/>
+        <v>1974834847</v>
+      </c>
+      <c r="J8" s="1">
         <v>6117361676</v>
       </c>
-      <c r="D8" s="1">
-        <v>1782428245</v>
-      </c>
-      <c r="E8" s="1">
-        <v>694920774</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="2">
-        <v>1957</v>
-      </c>
-      <c r="B9" s="1">
-        <v>12390940297</v>
-      </c>
-      <c r="C9" s="1">
-        <v>6924711381</v>
-      </c>
-      <c r="D9" s="1">
-        <v>2188653924</v>
-      </c>
-      <c r="E9" s="1">
-        <v>837606748</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10">
-        <v>1958</v>
-      </c>
-      <c r="B10" s="1">
-        <v>13709273168</v>
-      </c>
-      <c r="C10" s="1">
-        <v>7483340099</v>
-      </c>
-      <c r="D10" s="1">
-        <v>2336585079</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1164379666</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="2">
-        <v>1959</v>
-      </c>
-      <c r="B11" s="1">
-        <v>15611829655</v>
-      </c>
-      <c r="C11" s="1">
-        <v>7979676672</v>
-      </c>
-      <c r="D11" s="1">
-        <v>2800775826</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1338886027</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="2">
-        <v>1960</v>
-      </c>
-      <c r="B12" s="1">
-        <v>20659549782</v>
-      </c>
-      <c r="C12" s="1">
-        <v>11997894672</v>
-      </c>
-      <c r="D12" s="1">
-        <v>2863709505</v>
-      </c>
-      <c r="E12" s="1">
-        <v>1618128584</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13">
-        <v>1961</v>
-      </c>
-      <c r="B13" s="1">
-        <v>23186682768</v>
-      </c>
-      <c r="C13" s="1">
-        <v>13127507982</v>
-      </c>
-      <c r="D13" s="1">
-        <v>3471722192</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1724217344</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="2">
-        <v>1962</v>
-      </c>
-      <c r="B14" s="1">
-        <v>23406352096</v>
-      </c>
-      <c r="C14" s="1">
-        <v>12809779477</v>
-      </c>
-      <c r="D14" s="1">
-        <v>3327198494</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1995738863</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="2">
-        <v>1963</v>
-      </c>
-      <c r="B15" s="1">
-        <v>24508034204</v>
-      </c>
-      <c r="C15" s="1">
-        <v>12650218746</v>
-      </c>
-      <c r="D15" s="1">
-        <v>3707276007</v>
-      </c>
-      <c r="E15" s="1">
-        <v>2690631323</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B18" s="2" t="s">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="2"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="2"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="2"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="2"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="F18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2">
         <v>1950</v>
       </c>
       <c r="B19" s="4">
-        <f>B2/1000000</f>
-        <v>2786.7528339999999</v>
+        <f ca="1">C2/1000000</f>
+        <v>1255.12095</v>
       </c>
       <c r="C19" s="4">
-        <f t="shared" ref="C19:E19" si="0">C2/1000000</f>
-        <v>1553.185796</v>
+        <f ca="1">D2/1000000</f>
+        <v>298.06484599999999</v>
       </c>
       <c r="D19" s="4">
-        <f t="shared" si="0"/>
+        <f ca="1">E2/1000000</f>
         <v>523.64871600000004</v>
       </c>
       <c r="E19" s="4">
-        <f t="shared" si="0"/>
+        <f ca="1">F2/1000000</f>
         <v>297.153074</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F19" s="4">
+        <f ca="1">G2/1000000</f>
+        <v>0.22844800000000001</v>
+      </c>
+      <c r="G19" s="4">
+        <f ca="1">H2/1000000</f>
+        <v>412.53680000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>1951</v>
       </c>
       <c r="B20" s="4">
-        <f t="shared" ref="B20:E32" si="1">B3/1000000</f>
-        <v>3773.7650530000001</v>
+        <f ca="1">C3/1000000</f>
+        <v>1507.6941039999999</v>
       </c>
       <c r="C20" s="4">
-        <f t="shared" si="1"/>
-        <v>1925.545314</v>
+        <f ca="1">D3/1000000</f>
+        <v>417.85120999999998</v>
       </c>
       <c r="D20" s="4">
-        <f t="shared" si="1"/>
+        <f ca="1">E3/1000000</f>
         <v>748.33876299999997</v>
       </c>
       <c r="E20" s="4">
-        <f t="shared" si="1"/>
+        <f ca="1">F3/1000000</f>
         <v>423.51236499999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F20" s="4">
+        <f ca="1">G3/1000000</f>
+        <v>0.28353600000000001</v>
+      </c>
+      <c r="G20" s="4">
+        <f ca="1">H3/1000000</f>
+        <v>676.08507499999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2">
         <v>1952</v>
       </c>
       <c r="B21" s="4">
-        <f t="shared" si="1"/>
-        <v>5837.5524180000002</v>
+        <f ca="1">C4/1000000</f>
+        <v>2932.9228010000002</v>
       </c>
       <c r="C21" s="4">
-        <f t="shared" si="1"/>
-        <v>3596.1844769999998</v>
+        <f ca="1">D4/1000000</f>
+        <v>663.26167599999997</v>
       </c>
       <c r="D21" s="4">
-        <f t="shared" si="1"/>
+        <f ca="1">E4/1000000</f>
         <v>983.55200500000001</v>
       </c>
       <c r="E21" s="4">
-        <f t="shared" si="1"/>
+        <f ca="1">F4/1000000</f>
         <v>415.91105299999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F21" s="4">
+        <f ca="1">G4/1000000</f>
+        <v>0.79500400000000004</v>
+      </c>
+      <c r="G21" s="4">
+        <f ca="1">H4/1000000</f>
+        <v>841.10987899999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>1953</v>
       </c>
       <c r="B22" s="4">
-        <f t="shared" si="1"/>
-        <v>8681.4118269999999</v>
+        <f ca="1">C5/1000000</f>
+        <v>4577.1817259999998</v>
       </c>
       <c r="C22" s="4">
-        <f t="shared" si="1"/>
-        <v>5379.7804310000001</v>
+        <f ca="1">D5/1000000</f>
+        <v>802.598705</v>
       </c>
       <c r="D22" s="4">
-        <f t="shared" si="1"/>
+        <f ca="1">E5/1000000</f>
         <v>1638.0256770000001</v>
       </c>
       <c r="E22" s="4">
-        <f t="shared" si="1"/>
+        <f ca="1">F5/1000000</f>
         <v>452.49269800000002</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F22" s="4">
+        <f ca="1">G5/1000000</f>
+        <v>1.1640470000000001</v>
+      </c>
+      <c r="G22" s="4">
+        <f ca="1">H5/1000000</f>
+        <v>1209.9489739999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2">
         <v>1954</v>
       </c>
       <c r="B23" s="4">
-        <f t="shared" si="1"/>
-        <v>7430.6435419999998</v>
+        <f ca="1">C6/1000000</f>
+        <v>3531.8329450000001</v>
       </c>
       <c r="C23" s="4">
-        <f t="shared" si="1"/>
-        <v>4392.9813219999996</v>
+        <f ca="1">D6/1000000</f>
+        <v>861.14837699999998</v>
       </c>
       <c r="D23" s="4">
-        <f t="shared" si="1"/>
+        <f ca="1">E6/1000000</f>
         <v>1169.6238860000001</v>
       </c>
       <c r="E23" s="4">
-        <f t="shared" si="1"/>
+        <f ca="1">F6/1000000</f>
         <v>510.80731800000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F23" s="4">
+        <f ca="1">G6/1000000</f>
+        <v>1.1197649999999999</v>
+      </c>
+      <c r="G23" s="4">
+        <f ca="1">H6/1000000</f>
+        <v>1356.111251</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>1955</v>
       </c>
       <c r="B24" s="4">
-        <f t="shared" si="1"/>
-        <v>9494.8602339999998</v>
+        <f ca="1">C7/1000000</f>
+        <v>4357.2195009999996</v>
       </c>
       <c r="C24" s="4">
-        <f t="shared" si="1"/>
-        <v>5463.5659850000002</v>
+        <f ca="1">D7/1000000</f>
+        <v>1106.3464839999999</v>
       </c>
       <c r="D24" s="4">
-        <f t="shared" si="1"/>
+        <f ca="1">E7/1000000</f>
         <v>1623.1821150000001</v>
       </c>
       <c r="E24" s="4">
-        <f t="shared" si="1"/>
+        <f ca="1">F7/1000000</f>
         <v>630.16103199999998</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F24" s="4">
+        <f ca="1">G7/1000000</f>
+        <v>2.2695720000000001</v>
+      </c>
+      <c r="G24" s="4">
+        <f ca="1">H7/1000000</f>
+        <v>1775.6815300000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2">
         <v>1956</v>
       </c>
       <c r="B25" s="4">
-        <f t="shared" si="1"/>
-        <v>10574.045432000001</v>
+        <f ca="1">C8/1000000</f>
+        <v>4786.005365</v>
       </c>
       <c r="C25" s="4">
-        <f t="shared" si="1"/>
-        <v>6117.3616760000004</v>
+        <f ca="1">D8/1000000</f>
+        <v>1331.356311</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" si="1"/>
+        <f ca="1">E8/1000000</f>
         <v>1782.4282450000001</v>
       </c>
       <c r="E25" s="4">
-        <f t="shared" si="1"/>
+        <f ca="1">F8/1000000</f>
         <v>694.92077400000005</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26" s="2">
-        <v>1957</v>
-      </c>
-      <c r="B26" s="4">
-        <f t="shared" si="1"/>
-        <v>12390.940296999999</v>
-      </c>
-      <c r="C26" s="4">
-        <f t="shared" si="1"/>
-        <v>6924.7113810000001</v>
-      </c>
-      <c r="D26" s="4">
-        <f t="shared" si="1"/>
-        <v>2188.6539240000002</v>
-      </c>
-      <c r="E26" s="4">
-        <f t="shared" si="1"/>
-        <v>837.60674800000004</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A27">
-        <v>1958</v>
-      </c>
-      <c r="B27" s="4">
-        <f t="shared" si="1"/>
-        <v>13709.273168</v>
-      </c>
-      <c r="C27" s="4">
-        <f t="shared" si="1"/>
-        <v>7483.340099</v>
-      </c>
-      <c r="D27" s="4">
-        <f t="shared" si="1"/>
-        <v>2336.585079</v>
-      </c>
-      <c r="E27" s="4">
-        <f t="shared" si="1"/>
-        <v>1164.379666</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A28" s="2">
-        <v>1959</v>
-      </c>
-      <c r="B28" s="4">
-        <f t="shared" si="1"/>
-        <v>15611.829655</v>
-      </c>
-      <c r="C28" s="4">
-        <f t="shared" si="1"/>
-        <v>7979.6766719999996</v>
-      </c>
-      <c r="D28" s="4">
-        <f t="shared" si="1"/>
-        <v>2800.7758260000001</v>
-      </c>
-      <c r="E28" s="4">
-        <f t="shared" si="1"/>
-        <v>1338.886027</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A29" s="2">
-        <v>1960</v>
-      </c>
-      <c r="B29" s="4">
-        <f t="shared" si="1"/>
-        <v>20659.549781999998</v>
-      </c>
-      <c r="C29" s="4">
-        <f t="shared" si="1"/>
-        <v>11997.894672</v>
-      </c>
-      <c r="D29" s="4">
-        <f t="shared" si="1"/>
-        <v>2863.7095049999998</v>
-      </c>
-      <c r="E29" s="4">
-        <f t="shared" si="1"/>
-        <v>1618.128584</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A30">
-        <v>1961</v>
-      </c>
-      <c r="B30" s="4">
-        <f t="shared" si="1"/>
-        <v>23186.682767999999</v>
-      </c>
-      <c r="C30" s="4">
-        <f t="shared" si="1"/>
-        <v>13127.507981999999</v>
-      </c>
-      <c r="D30" s="4">
-        <f t="shared" si="1"/>
-        <v>3471.7221920000002</v>
-      </c>
-      <c r="E30" s="4">
-        <f t="shared" si="1"/>
-        <v>1724.2173439999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A31" s="2">
-        <v>1962</v>
-      </c>
-      <c r="B31" s="4">
-        <f t="shared" si="1"/>
-        <v>23406.352095999999</v>
-      </c>
-      <c r="C31" s="4">
-        <f t="shared" si="1"/>
-        <v>12809.779477</v>
-      </c>
-      <c r="D31" s="4">
-        <f t="shared" si="1"/>
-        <v>3327.1984940000002</v>
-      </c>
-      <c r="E31" s="4">
-        <f t="shared" si="1"/>
-        <v>1995.738863</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A32" s="2">
-        <v>1963</v>
-      </c>
-      <c r="B32" s="4">
-        <f t="shared" si="1"/>
-        <v>24508.034204</v>
-      </c>
-      <c r="C32" s="4">
-        <f t="shared" si="1"/>
-        <v>12650.218746</v>
-      </c>
-      <c r="D32" s="4">
-        <f t="shared" si="1"/>
-        <v>3707.2760069999999</v>
-      </c>
-      <c r="E32" s="4">
-        <f t="shared" si="1"/>
-        <v>2690.6313230000001</v>
-      </c>
+      <c r="F25" s="4">
+        <f ca="1">G8/1000000</f>
+        <v>4.4998899999999997</v>
+      </c>
+      <c r="G25" s="4">
+        <f ca="1">H8/1000000</f>
+        <v>1974.8348470000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="2"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="2"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="2"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="2"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="2"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>